<commit_message>
update function to get data from file
</commit_message>
<xml_diff>
--- a/Dialogue.xlsx
+++ b/Dialogue.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TelegramBOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\interactive_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21431024-F585-4ABA-9048-7FD761C62309}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1B9BA-89BD-408F-8B1B-1AB5F9523FB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861629FB-21DF-4EC3-8D07-ABA91F730913}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>user_id</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>group_id</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -418,126 +421,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F9A4D-1B6F-42D4-AD5F-3EDB965666D4}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>-1001158850531</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>-1001158850531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>-1001158850531</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add function to check user in group or not and join group
</commit_message>
<xml_diff>
--- a/Dialogue.xlsx
+++ b/Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\interactive_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1B9BA-89BD-408F-8B1B-1AB5F9523FB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4357FBE6-5401-4665-90DB-7633FF8A8EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861629FB-21DF-4EC3-8D07-ABA91F730913}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>user_id</t>
   </si>
@@ -421,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F9A4D-1B6F-42D4-AD5F-3EDB965666D4}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
   </cols>
@@ -574,6 +574,132 @@
         <v>-1001158850531</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>-1001159430667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>-1001159430667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add html page and handle login/register
</commit_message>
<xml_diff>
--- a/Dialogue.xlsx
+++ b/Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\interactive_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4357FBE6-5401-4665-90DB-7633FF8A8EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB59B1-981F-43E7-894A-5424610638F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861629FB-21DF-4EC3-8D07-ABA91F730913}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>user_id</t>
   </si>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F9A4D-1B6F-42D4-AD5F-3EDB965666D4}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,132 +574,6 @@
         <v>-1001158850531</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>-1001159430667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>-1001159430667</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update code with issue
</commit_message>
<xml_diff>
--- a/Dialogue.xlsx
+++ b/Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\interactive_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB59B1-981F-43E7-894A-5424610638F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E708B970-146E-4665-9E7A-03E834965B67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861629FB-21DF-4EC3-8D07-ABA91F730913}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A11" sqref="A11:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>